<commit_message>
0.10 read from excel
99% ready task
</commit_message>
<xml_diff>
--- a/task_1/persons.xlsx
+++ b/task_1/persons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Фамилия</t>
   </si>
@@ -38,22 +38,13 @@
     <t>Дата рождения</t>
   </si>
   <si>
-    <t>Зубец</t>
-  </si>
-  <si>
-    <t>Зуб</t>
-  </si>
-  <si>
-    <t>Зубович</t>
-  </si>
-  <si>
-    <t>Лекс</t>
-  </si>
-  <si>
-    <t>Лютор</t>
-  </si>
-  <si>
-    <t>Фак</t>
+    <t>Иванов</t>
+  </si>
+  <si>
+    <t>Илья</t>
+  </si>
+  <si>
+    <t>Михайлович</t>
   </si>
 </sst>
 </file>
@@ -376,11 +367,12 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -405,25 +397,20 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1">
-        <v>35411</v>
-      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1">
-        <v>35042</v>
+        <v>33433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>